<commit_message>
Add: Added some test data.
</commit_message>
<xml_diff>
--- a/tests/data/19880209/19880209_target_highlight.xlsx
+++ b/tests/data/19880209/19880209_target_highlight.xlsx
@@ -1,96 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dfd3df2fe22ca4a1/Workspace/consolidate_csv_to_excel/tests/data/19880209/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_73F29786B12B6EF3D0896511BAE194983F71D505" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{808A294D-A5BA-4A35-BF65-512695EBA089}"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="3840" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="8565" yWindow="3405" windowWidth="16410" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="target_0" sheetId="1" r:id="rId1"/>
-    <sheet name="target_1" sheetId="2" r:id="rId2"/>
-    <sheet name="target_2" sheetId="3" r:id="rId3"/>
-    <sheet name="target_3" sheetId="4" r:id="rId4"/>
-    <sheet name="no_csv" sheetId="6" r:id="rId5"/>
+    <sheet name="target_0" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="target_1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="target_2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="target_3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="no_csv" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
-  <si>
-    <t>Date_A</t>
-  </si>
-  <si>
-    <t>Date_B</t>
-  </si>
-  <si>
-    <t>Processing_Time</t>
-  </si>
-  <si>
-    <t>JSON</t>
-  </si>
-  <si>
-    <t>0s</t>
-  </si>
-  <si>
-    <t>[{"date_a": "1988-02-09T00:00:00", "date_b": "1988-02-09T00:00:00", "processing_time": "0s", "random_key": null}]</t>
-  </si>
-  <si>
-    <t>INVALID</t>
-  </si>
-  <si>
-    <t>2s</t>
-  </si>
-  <si>
-    <t>[{"date_a": "1988-02-08T23:59:59", "date_b": "1988-02-09T00:00:01", "processing_time": "2s", "random_key": true}]</t>
-  </si>
-  <si>
-    <t>4s</t>
-  </si>
-  <si>
-    <t>[{"date_a": "1988-02-08T23:59:58", "date_b": "1988-02-09T00:00:02", "processing_time": "4s", "random_key": null}]</t>
-  </si>
-  <si>
-    <t>6s</t>
-  </si>
-  <si>
-    <t>[{"date_a": "1988-02-08T23:59:57", "date_b": "1988-02-09T00:00:03", "processing_time": "6s", "random_key": true}]</t>
-  </si>
-  <si>
-    <t>No CSV file found.</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="游ゴシック"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="游ゴシック"/>
+      <charset val="128"/>
+      <family val="3"/>
       <sz val="6"/>
-      <name val="游ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -102,7 +50,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFBF7F"/>
+        <fgColor rgb="00FFFF7F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFBF7F"/>
       </patternFill>
     </fill>
   </fills>
@@ -118,34 +71,94 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -411,216 +424,285 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18.75"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date_A</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Date_B</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Processing_Time</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>JSON</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
         <v>32182</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="2" t="n">
         <v>32182</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3">
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>0s</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>[{"date_a": "1988-02-09T00:00:00", "date_b": "1988-02-09T00:00:00", "processing_time": "0s", "random_key": null}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
         <v>32182</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="3" t="n">
         <v>32182</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>INVALID</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>INVALID</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="FFFFFF7F"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18.75"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Date_A</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Date_B</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Processing_Time</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>JSON</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
         <v>32181.99998842593</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="2" t="n">
         <v>32182.00001157407</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>2s</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>[{"date_a": "1988-02-08T23:59:59", "date_b": "1988-02-09T00:00:01", "processing_time": "2s", "random_key": true}]</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="FFFFFF7F"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18.75"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3">
-        <v>32181.999305555561</v>
-      </c>
-      <c r="B2" s="3">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Date_A</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Date_B</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Processing_Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>JSON</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>32181.99930555556</v>
+      </c>
+      <c r="B2" s="3" t="n">
         <v>32182</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>4s</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>[{"date_a": "1988-02-08T23:59:58", "date_b": "1988-02-09T00:00:02", "processing_time": "4s", "random_key": null}]</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="FFFFFF7F"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18.75"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3">
-        <v>32181.999305555561</v>
-      </c>
-      <c r="B2" s="3">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Date_A</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Date_B</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Processing_Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>JSON</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>32181.99930555556</v>
+      </c>
+      <c r="B2" s="3" t="n">
         <v>32182</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>12</v>
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>6s</t>
+        </is>
+      </c>
+      <c r="D2" s="7" t="inlineStr">
+        <is>
+          <t>[{"date_a": "1988-02-08T23:59:57", "date_b": "1988-02-09T00:00:03", "processing_time": "6s", "random_key": true}]</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D196397-5433-48DF-8B99-6ED1AD216BCC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="FF7F7F7F"/>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18.75"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>13</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>No CSV file found.</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>